<commit_message>
Small changes to non-rafting experiment data
</commit_message>
<xml_diff>
--- a/NonRaftingCollisionModel/Data_ExperimentVsModel.xlsx
+++ b/NonRaftingCollisionModel/Data_ExperimentVsModel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25640" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="140">
   <si>
     <t>Condition</t>
   </si>
@@ -590,7 +590,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -631,6 +631,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -753,6 +755,12 @@
     <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -765,14 +773,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="Bad" xfId="39" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -794,6 +796,7 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -814,6 +817,7 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1149,7 +1153,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J62" sqref="J62"/>
+      <selection pane="bottomRight" activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1184,23 +1188,23 @@
       <c r="C1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="60" t="s">
+      <c r="E1" s="61"/>
+      <c r="F1" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60" t="s">
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="60" t="s">
+      <c r="J1" s="63"/>
+      <c r="K1" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="61"/>
+      <c r="L1" s="63"/>
       <c r="M1" s="38" t="s">
         <v>108</v>
       </c>
@@ -1213,17 +1217,17 @@
       <c r="P1" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="Q1" s="60" t="s">
+      <c r="Q1" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="59" t="s">
+      <c r="R1" s="62"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
       <c r="X1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1268,14 +1272,14 @@
       <c r="P2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Q2" s="58" t="s">
+      <c r="Q2" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58" t="s">
+      <c r="R2" s="60"/>
+      <c r="S2" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="T2" s="58"/>
+      <c r="T2" s="60"/>
       <c r="U2" s="3" t="s">
         <v>90</v>
       </c>
@@ -1382,25 +1386,25 @@
         <v>1</v>
       </c>
       <c r="H7" s="20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="31">
         <v>0</v>
       </c>
       <c r="J7" s="31">
-        <v>4.5400000000000003E-2</v>
+        <v>0.12609999999999999</v>
       </c>
       <c r="K7" s="22">
         <v>63</v>
       </c>
       <c r="L7" s="22">
-        <v>35.1</v>
+        <v>150.80000000000001</v>
       </c>
       <c r="M7" s="22">
         <v>12</v>
       </c>
-      <c r="N7" s="43" t="s">
-        <v>124</v>
+      <c r="N7" s="43">
+        <v>0.04</v>
       </c>
       <c r="O7" s="51">
         <v>0.72410473640434203</v>
@@ -1451,19 +1455,19 @@
         <v>7.3700000000000002E-2</v>
       </c>
       <c r="J8" s="31">
-        <v>6.2899999999999998E-2</v>
+        <v>0.13850000000000001</v>
       </c>
       <c r="K8" s="22">
         <v>51.4</v>
       </c>
       <c r="L8" s="22">
-        <v>25</v>
+        <v>79.2</v>
       </c>
       <c r="M8" s="22">
         <v>11</v>
       </c>
-      <c r="N8" s="43" t="s">
-        <v>124</v>
+      <c r="N8" s="43">
+        <v>0.04</v>
       </c>
       <c r="O8" s="51">
         <v>0.78903979340123298</v>
@@ -1514,19 +1518,19 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="J9" s="31">
-        <v>5.1400000000000001E-2</v>
+        <v>0.12859999999999999</v>
       </c>
       <c r="K9" s="22">
         <v>28.8</v>
       </c>
       <c r="L9" s="22">
-        <v>39.5</v>
+        <v>141.4</v>
       </c>
       <c r="M9" s="22">
         <v>8</v>
       </c>
-      <c r="N9" s="43" t="s">
-        <v>124</v>
+      <c r="N9" s="43">
+        <v>0.04</v>
       </c>
       <c r="O9" s="51">
         <v>0.78903979340123298</v>
@@ -2361,12 +2365,12 @@
       <c r="P22" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="Q22" s="62">
+      <c r="Q22" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R22" s="62"/>
-      <c r="S22" s="62">
+      <c r="R22" s="58"/>
+      <c r="S22" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2427,12 +2431,12 @@
       <c r="P23" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="Q23" s="62">
+      <c r="Q23" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R23" s="62"/>
-      <c r="S23" s="62">
+      <c r="R23" s="58"/>
+      <c r="S23" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2490,12 +2494,12 @@
       <c r="P24" s="51">
         <v>1.2445410250239799</v>
       </c>
-      <c r="Q24" s="62">
+      <c r="Q24" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R24" s="62"/>
-      <c r="S24" s="62">
+      <c r="R24" s="58"/>
+      <c r="S24" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2556,12 +2560,12 @@
       <c r="P25" s="51">
         <v>1.3545909310866799</v>
       </c>
-      <c r="Q25" s="62">
+      <c r="Q25" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R25" s="62"/>
-      <c r="S25" s="62">
+      <c r="R25" s="58"/>
+      <c r="S25" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2613,7 +2617,7 @@
       <c r="M26" s="22">
         <v>17</v>
       </c>
-      <c r="N26" s="63">
+      <c r="N26" s="59">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="O26" s="51">
@@ -2622,12 +2626,12 @@
       <c r="P26" s="51">
         <v>0.69236875802803499</v>
       </c>
-      <c r="Q26" s="62">
+      <c r="Q26" s="58">
         <f t="shared" si="0"/>
         <v>0.12967500000000001</v>
       </c>
-      <c r="R26" s="62"/>
-      <c r="S26" s="62">
+      <c r="R26" s="58"/>
+      <c r="S26" s="58">
         <f t="shared" si="1"/>
         <v>0.14332500000000001</v>
       </c>
@@ -4334,19 +4338,19 @@
         <v>0</v>
       </c>
       <c r="J57" s="29">
-        <v>8.6999999999999994E-2</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="K57" s="13">
         <v>119.64400000000001</v>
       </c>
       <c r="L57" s="56">
-        <v>44.8</v>
+        <v>111</v>
       </c>
       <c r="M57" s="13">
         <v>21.5</v>
       </c>
-      <c r="N57" s="40" t="s">
-        <v>139</v>
+      <c r="N57" s="40">
+        <v>0.04</v>
       </c>
       <c r="O57" s="48">
         <v>0.84199316147237901</v>
@@ -4430,14 +4434,18 @@
       <c r="I59" s="29">
         <v>0</v>
       </c>
-      <c r="J59" s="29"/>
+      <c r="J59" s="29">
+        <v>0.1242</v>
+      </c>
       <c r="K59" s="13">
         <v>89.631600000000006</v>
       </c>
-      <c r="L59" s="13"/>
+      <c r="L59" s="13">
+        <v>153.80000000000001</v>
+      </c>
       <c r="M59" s="13"/>
-      <c r="N59" s="40" t="s">
-        <v>139</v>
+      <c r="N59" s="40">
+        <v>0.04</v>
       </c>
       <c r="O59" s="48">
         <v>0.84199316147237901</v>
@@ -4550,7 +4558,9 @@
       <c r="J62" s="31"/>
       <c r="K62" s="22"/>
       <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
+      <c r="M62" s="22">
+        <v>23</v>
+      </c>
       <c r="N62" s="40" t="s">
         <v>139</v>
       </c>
@@ -4595,12 +4605,18 @@
       <c r="I63" s="29">
         <v>0</v>
       </c>
-      <c r="J63" s="29"/>
+      <c r="J63" s="29">
+        <v>0.1103</v>
+      </c>
       <c r="K63" s="13">
         <v>126.41160000000001</v>
       </c>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
+      <c r="L63" s="13">
+        <v>185.3</v>
+      </c>
+      <c r="M63" s="13">
+        <v>23</v>
+      </c>
       <c r="N63" s="40" t="s">
         <v>139</v>
       </c>

</xml_diff>